<commit_message>
credentials for db as env
</commit_message>
<xml_diff>
--- a/app/postgres_data/daily/DA_electricity/archiv/13_12_2022_DA_elec.xlsx
+++ b/app/postgres_data/daily/DA_electricity/archiv/13_12_2022_DA_elec.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="71">
   <si>
     <t>Datenkategorie: Großhandelspreise</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Zeitraum: 28.11.2022, 00:00 - 15.12.2022, 23:59</t>
   </si>
   <si>
-    <t>Stand: 13.12.2022, 13:19</t>
+    <t>Stand: 13.12.2022, 16:14</t>
   </si>
   <si>
     <t>(c) Bundesnetzagentur | SMARD.de</t>
@@ -24200,8 +24200,8 @@
       <c r="D395" t="n" s="1">
         <v>274.82</v>
       </c>
-      <c r="E395" t="s">
-        <v>31</v>
+      <c r="E395" t="n" s="1">
+        <v>285.41</v>
       </c>
       <c r="F395" t="n" s="1">
         <v>325.0</v>
@@ -24230,8 +24230,8 @@
       <c r="N395" t="n" s="1">
         <v>271.89</v>
       </c>
-      <c r="O395" t="s">
-        <v>31</v>
+      <c r="O395" t="n" s="1">
+        <v>344.93</v>
       </c>
       <c r="P395" t="n" s="1">
         <v>273.94</v>
@@ -24239,8 +24239,8 @@
       <c r="Q395" t="s">
         <v>31</v>
       </c>
-      <c r="R395" t="s">
-        <v>31</v>
+      <c r="R395" t="n" s="1">
+        <v>338.37</v>
       </c>
       <c r="S395" t="n" s="1">
         <v>293.1</v>
@@ -24262,8 +24262,8 @@
       <c r="D396" t="n" s="1">
         <v>270.47</v>
       </c>
-      <c r="E396" t="s">
-        <v>31</v>
+      <c r="E396" t="n" s="1">
+        <v>275.89</v>
       </c>
       <c r="F396" t="n" s="1">
         <v>299.95</v>
@@ -24292,8 +24292,8 @@
       <c r="N396" t="n" s="1">
         <v>270.47</v>
       </c>
-      <c r="O396" t="s">
-        <v>31</v>
+      <c r="O396" t="n" s="1">
+        <v>320.03</v>
       </c>
       <c r="P396" t="n" s="1">
         <v>269.16</v>
@@ -24301,8 +24301,8 @@
       <c r="Q396" t="s">
         <v>31</v>
       </c>
-      <c r="R396" t="s">
-        <v>31</v>
+      <c r="R396" t="n" s="1">
+        <v>321.0</v>
       </c>
       <c r="S396" t="n" s="1">
         <v>283.34</v>
@@ -24324,8 +24324,8 @@
       <c r="D397" t="n" s="1">
         <v>268.69</v>
       </c>
-      <c r="E397" t="s">
-        <v>31</v>
+      <c r="E397" t="n" s="1">
+        <v>275.05</v>
       </c>
       <c r="F397" t="n" s="1">
         <v>301.08</v>
@@ -24354,8 +24354,8 @@
       <c r="N397" t="n" s="1">
         <v>268.69</v>
       </c>
-      <c r="O397" t="s">
-        <v>31</v>
+      <c r="O397" t="n" s="1">
+        <v>306.49</v>
       </c>
       <c r="P397" t="n" s="1">
         <v>267.17</v>
@@ -24363,8 +24363,8 @@
       <c r="Q397" t="s">
         <v>31</v>
       </c>
-      <c r="R397" t="s">
-        <v>31</v>
+      <c r="R397" t="n" s="1">
+        <v>306.54</v>
       </c>
       <c r="S397" t="n" s="1">
         <v>283.02</v>
@@ -24386,8 +24386,8 @@
       <c r="D398" t="n" s="1">
         <v>278.2</v>
       </c>
-      <c r="E398" t="s">
-        <v>31</v>
+      <c r="E398" t="n" s="1">
+        <v>273.63</v>
       </c>
       <c r="F398" t="n" s="1">
         <v>285.25</v>
@@ -24416,8 +24416,8 @@
       <c r="N398" t="n" s="1">
         <v>278.0</v>
       </c>
-      <c r="O398" t="s">
-        <v>31</v>
+      <c r="O398" t="n" s="1">
+        <v>293.08</v>
       </c>
       <c r="P398" t="n" s="1">
         <v>277.98</v>
@@ -24425,8 +24425,8 @@
       <c r="Q398" t="s">
         <v>31</v>
       </c>
-      <c r="R398" t="s">
-        <v>31</v>
+      <c r="R398" t="n" s="1">
+        <v>289.36</v>
       </c>
       <c r="S398" t="n" s="1">
         <v>281.05</v>
@@ -24448,8 +24448,8 @@
       <c r="D399" t="n" s="1">
         <v>280.21</v>
       </c>
-      <c r="E399" t="s">
-        <v>31</v>
+      <c r="E399" t="n" s="1">
+        <v>274.28</v>
       </c>
       <c r="F399" t="n" s="1">
         <v>287.47</v>
@@ -24478,8 +24478,8 @@
       <c r="N399" t="n" s="1">
         <v>279.69</v>
       </c>
-      <c r="O399" t="s">
-        <v>31</v>
+      <c r="O399" t="n" s="1">
+        <v>285.56</v>
       </c>
       <c r="P399" t="n" s="1">
         <v>279.88</v>
@@ -24487,8 +24487,8 @@
       <c r="Q399" t="s">
         <v>31</v>
       </c>
-      <c r="R399" t="s">
-        <v>31</v>
+      <c r="R399" t="n" s="1">
+        <v>292.79</v>
       </c>
       <c r="S399" t="n" s="1">
         <v>283.42</v>
@@ -24510,8 +24510,8 @@
       <c r="D400" t="n" s="1">
         <v>311.11</v>
       </c>
-      <c r="E400" t="s">
-        <v>31</v>
+      <c r="E400" t="n" s="1">
+        <v>300.11</v>
       </c>
       <c r="F400" t="n" s="1">
         <v>313.0</v>
@@ -24540,8 +24540,8 @@
       <c r="N400" t="n" s="1">
         <v>311.11</v>
       </c>
-      <c r="O400" t="s">
-        <v>31</v>
+      <c r="O400" t="n" s="1">
+        <v>312.84</v>
       </c>
       <c r="P400" t="n" s="1">
         <v>311.23</v>
@@ -24549,8 +24549,8 @@
       <c r="Q400" t="s">
         <v>31</v>
       </c>
-      <c r="R400" t="s">
-        <v>31</v>
+      <c r="R400" t="n" s="1">
+        <v>312.14</v>
       </c>
       <c r="S400" t="n" s="1">
         <v>311.37</v>
@@ -24572,8 +24572,8 @@
       <c r="D401" t="n" s="1">
         <v>368.82</v>
       </c>
-      <c r="E401" t="s">
-        <v>31</v>
+      <c r="E401" t="n" s="1">
+        <v>352.27</v>
       </c>
       <c r="F401" t="n" s="1">
         <v>368.82</v>
@@ -24602,8 +24602,8 @@
       <c r="N401" t="n" s="1">
         <v>368.82</v>
       </c>
-      <c r="O401" t="s">
-        <v>31</v>
+      <c r="O401" t="n" s="1">
+        <v>366.1</v>
       </c>
       <c r="P401" t="n" s="1">
         <v>368.82</v>
@@ -24611,8 +24611,8 @@
       <c r="Q401" t="s">
         <v>31</v>
       </c>
-      <c r="R401" t="s">
-        <v>31</v>
+      <c r="R401" t="n" s="1">
+        <v>368.82</v>
       </c>
       <c r="S401" t="n" s="1">
         <v>368.82</v>
@@ -24634,8 +24634,8 @@
       <c r="D402" t="n" s="1">
         <v>494.97</v>
       </c>
-      <c r="E402" t="s">
-        <v>31</v>
+      <c r="E402" t="n" s="1">
+        <v>465.75</v>
       </c>
       <c r="F402" t="n" s="1">
         <v>494.97</v>
@@ -24664,8 +24664,8 @@
       <c r="N402" t="n" s="1">
         <v>494.97</v>
       </c>
-      <c r="O402" t="s">
-        <v>31</v>
+      <c r="O402" t="n" s="1">
+        <v>474.26</v>
       </c>
       <c r="P402" t="n" s="1">
         <v>494.97</v>
@@ -24673,8 +24673,8 @@
       <c r="Q402" t="s">
         <v>31</v>
       </c>
-      <c r="R402" t="s">
-        <v>31</v>
+      <c r="R402" t="n" s="1">
+        <v>494.97</v>
       </c>
       <c r="S402" t="n" s="1">
         <v>494.97</v>
@@ -24696,8 +24696,8 @@
       <c r="D403" t="n" s="1">
         <v>539.99</v>
       </c>
-      <c r="E403" t="s">
-        <v>31</v>
+      <c r="E403" t="n" s="1">
+        <v>508.64</v>
       </c>
       <c r="F403" t="n" s="1">
         <v>539.99</v>
@@ -24726,8 +24726,8 @@
       <c r="N403" t="n" s="1">
         <v>539.99</v>
       </c>
-      <c r="O403" t="s">
-        <v>31</v>
+      <c r="O403" t="n" s="1">
+        <v>529.26</v>
       </c>
       <c r="P403" t="n" s="1">
         <v>539.99</v>
@@ -24735,8 +24735,8 @@
       <c r="Q403" t="s">
         <v>31</v>
       </c>
-      <c r="R403" t="s">
-        <v>31</v>
+      <c r="R403" t="n" s="1">
+        <v>539.99</v>
       </c>
       <c r="S403" t="n" s="1">
         <v>539.99</v>
@@ -24758,8 +24758,8 @@
       <c r="D404" t="n" s="1">
         <v>569.72</v>
       </c>
-      <c r="E404" t="s">
-        <v>31</v>
+      <c r="E404" t="n" s="1">
+        <v>532.9</v>
       </c>
       <c r="F404" t="n" s="1">
         <v>569.72</v>
@@ -24788,8 +24788,8 @@
       <c r="N404" t="n" s="1">
         <v>569.72</v>
       </c>
-      <c r="O404" t="s">
-        <v>31</v>
+      <c r="O404" t="n" s="1">
+        <v>530.72</v>
       </c>
       <c r="P404" t="n" s="1">
         <v>569.72</v>
@@ -24797,8 +24797,8 @@
       <c r="Q404" t="s">
         <v>31</v>
       </c>
-      <c r="R404" t="s">
-        <v>31</v>
+      <c r="R404" t="n" s="1">
+        <v>569.72</v>
       </c>
       <c r="S404" t="n" s="1">
         <v>569.72</v>
@@ -24820,8 +24820,8 @@
       <c r="D405" t="n" s="1">
         <v>565.18</v>
       </c>
-      <c r="E405" t="s">
-        <v>31</v>
+      <c r="E405" t="n" s="1">
+        <v>527.44</v>
       </c>
       <c r="F405" t="n" s="1">
         <v>565.18</v>
@@ -24850,8 +24850,8 @@
       <c r="N405" t="n" s="1">
         <v>565.18</v>
       </c>
-      <c r="O405" t="s">
-        <v>31</v>
+      <c r="O405" t="n" s="1">
+        <v>518.79</v>
       </c>
       <c r="P405" t="n" s="1">
         <v>565.18</v>
@@ -24859,8 +24859,8 @@
       <c r="Q405" t="s">
         <v>31</v>
       </c>
-      <c r="R405" t="s">
-        <v>31</v>
+      <c r="R405" t="n" s="1">
+        <v>565.18</v>
       </c>
       <c r="S405" t="n" s="1">
         <v>565.18</v>
@@ -24882,8 +24882,8 @@
       <c r="D406" t="n" s="1">
         <v>568.01</v>
       </c>
-      <c r="E406" t="s">
-        <v>31</v>
+      <c r="E406" t="n" s="1">
+        <v>530.14</v>
       </c>
       <c r="F406" t="n" s="1">
         <v>568.01</v>
@@ -24912,8 +24912,8 @@
       <c r="N406" t="n" s="1">
         <v>568.01</v>
       </c>
-      <c r="O406" t="s">
-        <v>31</v>
+      <c r="O406" t="n" s="1">
+        <v>511.88</v>
       </c>
       <c r="P406" t="n" s="1">
         <v>568.01</v>
@@ -24921,8 +24921,8 @@
       <c r="Q406" t="s">
         <v>31</v>
       </c>
-      <c r="R406" t="s">
-        <v>31</v>
+      <c r="R406" t="n" s="1">
+        <v>568.01</v>
       </c>
       <c r="S406" t="n" s="1">
         <v>568.01</v>
@@ -24944,8 +24944,8 @@
       <c r="D407" t="n" s="1">
         <v>526.07</v>
       </c>
-      <c r="E407" t="s">
-        <v>31</v>
+      <c r="E407" t="n" s="1">
+        <v>485.04</v>
       </c>
       <c r="F407" t="n" s="1">
         <v>503.85</v>
@@ -24974,8 +24974,8 @@
       <c r="N407" t="n" s="1">
         <v>526.1</v>
       </c>
-      <c r="O407" t="s">
-        <v>31</v>
+      <c r="O407" t="n" s="1">
+        <v>501.9</v>
       </c>
       <c r="P407" t="n" s="1">
         <v>524.6</v>
@@ -24983,8 +24983,8 @@
       <c r="Q407" t="s">
         <v>31</v>
       </c>
-      <c r="R407" t="s">
-        <v>31</v>
+      <c r="R407" t="n" s="1">
+        <v>511.08</v>
       </c>
       <c r="S407" t="n" s="1">
         <v>521.39</v>
@@ -25006,8 +25006,8 @@
       <c r="D408" t="n" s="1">
         <v>515.48</v>
       </c>
-      <c r="E408" t="s">
-        <v>31</v>
+      <c r="E408" t="n" s="1">
+        <v>477.47</v>
       </c>
       <c r="F408" t="n" s="1">
         <v>494.7</v>
@@ -25036,8 +25036,8 @@
       <c r="N408" t="n" s="1">
         <v>515.73</v>
       </c>
-      <c r="O408" t="s">
-        <v>31</v>
+      <c r="O408" t="n" s="1">
+        <v>499.18</v>
       </c>
       <c r="P408" t="n" s="1">
         <v>514.16</v>
@@ -25045,8 +25045,8 @@
       <c r="Q408" t="s">
         <v>31</v>
       </c>
-      <c r="R408" t="s">
-        <v>31</v>
+      <c r="R408" t="n" s="1">
+        <v>501.34</v>
       </c>
       <c r="S408" t="n" s="1">
         <v>511.3</v>
@@ -25068,8 +25068,8 @@
       <c r="D409" t="n" s="1">
         <v>514.95</v>
       </c>
-      <c r="E409" t="s">
-        <v>31</v>
+      <c r="E409" t="n" s="1">
+        <v>488.19</v>
       </c>
       <c r="F409" t="n" s="1">
         <v>514.95</v>
@@ -25098,8 +25098,8 @@
       <c r="N409" t="n" s="1">
         <v>514.95</v>
       </c>
-      <c r="O409" t="s">
-        <v>31</v>
+      <c r="O409" t="n" s="1">
+        <v>518.08</v>
       </c>
       <c r="P409" t="n" s="1">
         <v>514.95</v>
@@ -25107,8 +25107,8 @@
       <c r="Q409" t="s">
         <v>31</v>
       </c>
-      <c r="R409" t="s">
-        <v>31</v>
+      <c r="R409" t="n" s="1">
+        <v>514.95</v>
       </c>
       <c r="S409" t="n" s="1">
         <v>514.95</v>
@@ -25130,8 +25130,8 @@
       <c r="D410" t="n" s="1">
         <v>528.53</v>
       </c>
-      <c r="E410" t="s">
-        <v>31</v>
+      <c r="E410" t="n" s="1">
+        <v>499.67</v>
       </c>
       <c r="F410" t="n" s="1">
         <v>528.53</v>
@@ -25160,8 +25160,8 @@
       <c r="N410" t="n" s="1">
         <v>528.53</v>
       </c>
-      <c r="O410" t="s">
-        <v>31</v>
+      <c r="O410" t="n" s="1">
+        <v>526.34</v>
       </c>
       <c r="P410" t="n" s="1">
         <v>528.53</v>
@@ -25169,8 +25169,8 @@
       <c r="Q410" t="s">
         <v>31</v>
       </c>
-      <c r="R410" t="s">
-        <v>31</v>
+      <c r="R410" t="n" s="1">
+        <v>528.53</v>
       </c>
       <c r="S410" t="n" s="1">
         <v>528.53</v>
@@ -25192,8 +25192,8 @@
       <c r="D411" t="n" s="1">
         <v>545.0</v>
       </c>
-      <c r="E411" t="s">
-        <v>31</v>
+      <c r="E411" t="n" s="1">
+        <v>513.96</v>
       </c>
       <c r="F411" t="n" s="1">
         <v>545.0</v>
@@ -25222,8 +25222,8 @@
       <c r="N411" t="n" s="1">
         <v>545.0</v>
       </c>
-      <c r="O411" t="s">
-        <v>31</v>
+      <c r="O411" t="n" s="1">
+        <v>534.8</v>
       </c>
       <c r="P411" t="n" s="1">
         <v>545.0</v>
@@ -25231,8 +25231,8 @@
       <c r="Q411" t="s">
         <v>31</v>
       </c>
-      <c r="R411" t="s">
-        <v>31</v>
+      <c r="R411" t="n" s="1">
+        <v>545.0</v>
       </c>
       <c r="S411" t="n" s="1">
         <v>545.0</v>
@@ -25254,8 +25254,8 @@
       <c r="D412" t="n" s="1">
         <v>590.0</v>
       </c>
-      <c r="E412" t="s">
-        <v>31</v>
+      <c r="E412" t="n" s="1">
+        <v>555.1</v>
       </c>
       <c r="F412" t="n" s="1">
         <v>590.0</v>
@@ -25284,8 +25284,8 @@
       <c r="N412" t="n" s="1">
         <v>590.0</v>
       </c>
-      <c r="O412" t="s">
-        <v>31</v>
+      <c r="O412" t="n" s="1">
+        <v>581.72</v>
       </c>
       <c r="P412" t="n" s="1">
         <v>590.0</v>
@@ -25293,8 +25293,8 @@
       <c r="Q412" t="s">
         <v>31</v>
       </c>
-      <c r="R412" t="s">
-        <v>31</v>
+      <c r="R412" t="n" s="1">
+        <v>590.0</v>
       </c>
       <c r="S412" t="n" s="1">
         <v>590.0</v>
@@ -25316,8 +25316,8 @@
       <c r="D413" t="n" s="1">
         <v>557.0</v>
       </c>
-      <c r="E413" t="s">
-        <v>31</v>
+      <c r="E413" t="n" s="1">
+        <v>525.21</v>
       </c>
       <c r="F413" t="n" s="1">
         <v>557.0</v>
@@ -25346,8 +25346,8 @@
       <c r="N413" t="n" s="1">
         <v>557.0</v>
       </c>
-      <c r="O413" t="s">
-        <v>31</v>
+      <c r="O413" t="n" s="1">
+        <v>556.59</v>
       </c>
       <c r="P413" t="n" s="1">
         <v>557.0</v>
@@ -25355,8 +25355,8 @@
       <c r="Q413" t="s">
         <v>31</v>
       </c>
-      <c r="R413" t="s">
-        <v>31</v>
+      <c r="R413" t="n" s="1">
+        <v>557.0</v>
       </c>
       <c r="S413" t="n" s="1">
         <v>557.0</v>
@@ -25378,8 +25378,8 @@
       <c r="D414" t="n" s="1">
         <v>520.57</v>
       </c>
-      <c r="E414" t="s">
-        <v>31</v>
+      <c r="E414" t="n" s="1">
+        <v>490.86</v>
       </c>
       <c r="F414" t="n" s="1">
         <v>520.57</v>
@@ -25408,8 +25408,8 @@
       <c r="N414" t="n" s="1">
         <v>520.57</v>
       </c>
-      <c r="O414" t="s">
-        <v>31</v>
+      <c r="O414" t="n" s="1">
+        <v>514.89</v>
       </c>
       <c r="P414" t="n" s="1">
         <v>520.57</v>
@@ -25417,8 +25417,8 @@
       <c r="Q414" t="s">
         <v>31</v>
       </c>
-      <c r="R414" t="s">
-        <v>31</v>
+      <c r="R414" t="n" s="1">
+        <v>520.57</v>
       </c>
       <c r="S414" t="n" s="1">
         <v>520.57</v>
@@ -25440,8 +25440,8 @@
       <c r="D415" t="n" s="1">
         <v>487.9</v>
       </c>
-      <c r="E415" t="s">
-        <v>31</v>
+      <c r="E415" t="n" s="1">
+        <v>458.83</v>
       </c>
       <c r="F415" t="n" s="1">
         <v>487.9</v>
@@ -25470,8 +25470,8 @@
       <c r="N415" t="n" s="1">
         <v>487.9</v>
       </c>
-      <c r="O415" t="s">
-        <v>31</v>
+      <c r="O415" t="n" s="1">
+        <v>463.17</v>
       </c>
       <c r="P415" t="n" s="1">
         <v>487.9</v>
@@ -25479,8 +25479,8 @@
       <c r="Q415" t="s">
         <v>31</v>
       </c>
-      <c r="R415" t="s">
-        <v>31</v>
+      <c r="R415" t="n" s="1">
+        <v>487.9</v>
       </c>
       <c r="S415" t="n" s="1">
         <v>487.9</v>
@@ -25502,8 +25502,8 @@
       <c r="D416" t="n" s="1">
         <v>396.67</v>
       </c>
-      <c r="E416" t="s">
-        <v>31</v>
+      <c r="E416" t="n" s="1">
+        <v>376.37</v>
       </c>
       <c r="F416" t="n" s="1">
         <v>396.67</v>
@@ -25532,8 +25532,8 @@
       <c r="N416" t="n" s="1">
         <v>396.67</v>
       </c>
-      <c r="O416" t="s">
-        <v>31</v>
+      <c r="O416" t="n" s="1">
+        <v>393.79</v>
       </c>
       <c r="P416" t="n" s="1">
         <v>396.67</v>
@@ -25541,8 +25541,8 @@
       <c r="Q416" t="s">
         <v>31</v>
       </c>
-      <c r="R416" t="s">
-        <v>31</v>
+      <c r="R416" t="n" s="1">
+        <v>396.67</v>
       </c>
       <c r="S416" t="n" s="1">
         <v>396.67</v>
@@ -25564,8 +25564,8 @@
       <c r="D417" t="n" s="1">
         <v>351.72</v>
       </c>
-      <c r="E417" t="s">
-        <v>31</v>
+      <c r="E417" t="n" s="1">
+        <v>336.99</v>
       </c>
       <c r="F417" t="n" s="1">
         <v>351.72</v>
@@ -25594,8 +25594,8 @@
       <c r="N417" t="n" s="1">
         <v>351.72</v>
       </c>
-      <c r="O417" t="s">
-        <v>31</v>
+      <c r="O417" t="n" s="1">
+        <v>356.91</v>
       </c>
       <c r="P417" t="n" s="1">
         <v>351.72</v>
@@ -25603,8 +25603,8 @@
       <c r="Q417" t="s">
         <v>31</v>
       </c>
-      <c r="R417" t="s">
-        <v>31</v>
+      <c r="R417" t="n" s="1">
+        <v>351.72</v>
       </c>
       <c r="S417" t="n" s="1">
         <v>351.72</v>
@@ -25626,8 +25626,8 @@
       <c r="D418" t="n" s="1">
         <v>328.94</v>
       </c>
-      <c r="E418" t="s">
-        <v>31</v>
+      <c r="E418" t="n" s="1">
+        <v>316.37</v>
       </c>
       <c r="F418" t="n" s="1">
         <v>342.0</v>
@@ -25656,8 +25656,8 @@
       <c r="N418" t="n" s="1">
         <v>328.94</v>
       </c>
-      <c r="O418" t="s">
-        <v>31</v>
+      <c r="O418" t="n" s="1">
+        <v>336.65</v>
       </c>
       <c r="P418" t="n" s="1">
         <v>328.75</v>
@@ -25665,8 +25665,8 @@
       <c r="Q418" t="s">
         <v>31</v>
       </c>
-      <c r="R418" t="s">
-        <v>31</v>
+      <c r="R418" t="n" s="1">
+        <v>336.28</v>
       </c>
       <c r="S418" t="n" s="1">
         <v>336.28</v>

</xml_diff>